<commit_message>
db env variables in config
</commit_message>
<xml_diff>
--- a/uploads/jira_description.xlsx
+++ b/uploads/jira_description.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="57">
   <si>
     <t>Ticket</t>
   </si>
@@ -31,12 +31,18 @@
     <t>Action</t>
   </si>
   <si>
-    <t>RuleType</t>
-  </si>
-  <si>
     <t>Entity</t>
   </si>
   <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>TargetDBsource</t>
+  </si>
+  <si>
+    <t>WrapperQuery</t>
+  </si>
+  <si>
     <t>PDM-12345</t>
   </si>
   <si>
@@ -52,21 +58,18 @@
     <t>Add</t>
   </si>
   <si>
-    <t>Mandatory</t>
-  </si>
-  <si>
     <t>org</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>PDM-12348</t>
   </si>
   <si>
     <t>DQ1649</t>
   </si>
   <si>
-    <t>Query</t>
-  </si>
-  <si>
     <t>pract</t>
   </si>
   <si>
@@ -103,22 +106,85 @@
     <t>PDM-12357</t>
   </si>
   <si>
+    <t>hf</t>
+  </si>
+  <si>
     <t>DQ1234</t>
   </si>
   <si>
     <t>Missing Processing Action Source Validation</t>
   </si>
   <si>
-    <t>Update</t>
+    <t>Configure</t>
+  </si>
+  <si>
+    <t>ATLAS</t>
+  </si>
+  <si>
+    <t>schema.table.column</t>
+  </si>
+  <si>
+    <t>PDM-12358</t>
+  </si>
+  <si>
+    <t>ROSTER</t>
+  </si>
+  <si>
+    <t>PDM-12359</t>
+  </si>
+  <si>
+    <t>DQ1235</t>
+  </si>
+  <si>
+    <t>Missing Processing Action Status Validation</t>
+  </si>
+  <si>
+    <t>PDM-12360</t>
+  </si>
+  <si>
+    <t>PDM-12361</t>
+  </si>
+  <si>
+    <t>DQ1233</t>
+  </si>
+  <si>
+    <t>Missing Processing Action Effective Start Date Validation</t>
   </si>
   <si>
     <t>PDM-12362</t>
   </si>
   <si>
-    <t>DQ1233</t>
-  </si>
-  <si>
-    <t>Missing Processing Action Effective Start Date Validation</t>
+    <t>PDM-12363</t>
+  </si>
+  <si>
+    <t>DQ1083</t>
+  </si>
+  <si>
+    <t>PDM-12364</t>
+  </si>
+  <si>
+    <t>PDM-12365</t>
+  </si>
+  <si>
+    <t>DQ1084</t>
+  </si>
+  <si>
+    <t>Missing Processing Action Source validation (Warning)</t>
+  </si>
+  <si>
+    <t>PDM-12366</t>
+  </si>
+  <si>
+    <t>PDM-12367</t>
+  </si>
+  <si>
+    <t>DQ1085</t>
+  </si>
+  <si>
+    <t>Missing Processing Action Status validation</t>
+  </si>
+  <si>
+    <t>PDM-12368</t>
   </si>
 </sst>
 </file>
@@ -169,12 +235,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -482,19 +551,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="61.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="61.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="8.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -513,195 +584,483 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>13</v>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>